<commit_message>
update cide xls sheets
</commit_message>
<xml_diff>
--- a/data/SJ_Codes_wb.xlsx
+++ b/data/SJ_Codes_wb.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stats\Test data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Watir\Watir_Sandbox\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
-  <si>
-    <t>Code</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>100000004snj</t>
   </si>
@@ -879,10 +876,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A19"/>
+  <dimension ref="A1:A18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -917,7 +914,7 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
@@ -978,11 +975,6 @@
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>